<commit_message>
added analysis of AAK1
</commit_message>
<xml_diff>
--- a/Blood cancer/output/gene_data1.xlsx
+++ b/Blood cancer/output/gene_data1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">GeneSymbol</t>
   </si>
@@ -150,6 +150,126 @@
   </si>
   <si>
     <t xml:space="preserve">ENSG00000107362.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000121410.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AACSP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000250420.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAGAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000103591.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAMDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000087884.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000090861.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABALON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000281376.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000167972.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCA8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000141338.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCB10P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000274099.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCB10P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000261524.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCB10P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000260053.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCB6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000115657.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCB8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000197150.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000125257.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000033050.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHD11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000106077.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000011198.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000175164.13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000146109.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC000041.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENSG00000242156.1</t>
   </si>
 </sst>
 </file>
@@ -903,402 +1023,402 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C22" t="n">
-        <v>9.24</v>
+        <v>6.45</v>
       </c>
       <c r="D22" t="n">
-        <v>2.895</v>
+        <v>18.61</v>
       </c>
       <c r="E22" t="n">
-        <v>1.394</v>
+        <v>-1.396</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0000000000000000000000000000000000013</v>
+        <v>0.00000000000000000000000000000401</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C23" t="n">
-        <v>3.02</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.515</v>
+        <v>2.535</v>
       </c>
       <c r="E23" t="n">
-        <v>1.408</v>
+        <v>-1.822</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0000000000000000000119</v>
+        <v>4.1e-229</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C24" t="n">
-        <v>2.16</v>
+        <v>20.52</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>52.548</v>
       </c>
       <c r="E24" t="n">
-        <v>1.66</v>
+        <v>-1.315</v>
       </c>
       <c r="F24" t="n">
-        <v>0.000000000000000000000000000000000000672</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000398</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C25" t="n">
-        <v>55.981</v>
+        <v>13.39</v>
       </c>
       <c r="D25" t="n">
-        <v>8.71</v>
+        <v>28.505</v>
       </c>
       <c r="E25" t="n">
-        <v>2.553</v>
+        <v>-1.036</v>
       </c>
       <c r="F25" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000128</v>
+        <v>0.000000000000000000000000000000000000000000000000366</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C26" t="n">
-        <v>4.13</v>
+        <v>31.441</v>
       </c>
       <c r="D26" t="n">
-        <v>0.565</v>
+        <v>205.329</v>
       </c>
       <c r="E26" t="n">
-        <v>1.713</v>
+        <v>-2.669</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0000000000000000000000000000000000000000456</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000238</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C27" t="n">
-        <v>7.83</v>
+        <v>0.96</v>
       </c>
       <c r="D27" t="n">
-        <v>0.175</v>
+        <v>3.3</v>
       </c>
       <c r="E27" t="n">
-        <v>2.91</v>
+        <v>-1.133</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000481</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000128</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C28" t="n">
-        <v>3.81</v>
+        <v>2.38</v>
       </c>
       <c r="D28" t="n">
-        <v>0.02</v>
+        <v>7.385</v>
       </c>
       <c r="E28" t="n">
-        <v>2.237</v>
+        <v>-1.311</v>
       </c>
       <c r="F28" t="n">
-        <v>0.00000000000000000000000000000000000000000000000513</v>
+        <v>0.00000000000000000000000264</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C29" t="n">
-        <v>48.86</v>
+        <v>0.16</v>
       </c>
       <c r="D29" t="n">
-        <v>15.95</v>
+        <v>12.8</v>
       </c>
       <c r="E29" t="n">
-        <v>1.557</v>
+        <v>-3.572</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0000000000000000000532</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000231</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C30" t="n">
-        <v>6.07</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>1.535</v>
+        <v>2.75</v>
       </c>
       <c r="E30" t="n">
-        <v>1.48</v>
+        <v>-1.907</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0000000000000000000000979</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000012</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C31" t="n">
-        <v>2.53</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.285</v>
+        <v>10.505</v>
       </c>
       <c r="E31" t="n">
-        <v>1.458</v>
+        <v>-3.524</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0000000000000000000264</v>
+        <v>4.13e-251</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C32" t="n">
-        <v>54.191</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>20.569</v>
+        <v>25.325</v>
       </c>
       <c r="E32" t="n">
-        <v>1.355</v>
+        <v>-4.718</v>
       </c>
       <c r="F32" t="n">
-        <v>0.000000000000000000000000357</v>
+        <v>1.42e-256</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C33" t="n">
-        <v>1.11</v>
+        <v>5.31</v>
       </c>
       <c r="D33" t="n">
-        <v>0.05</v>
+        <v>20.2</v>
       </c>
       <c r="E33" t="n">
-        <v>1.007</v>
+        <v>-1.748</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000234</v>
+        <v>0.00000000000000000000000000000134</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C34" t="n">
-        <v>5.18</v>
+        <v>18.02</v>
       </c>
       <c r="D34" t="n">
-        <v>0.195</v>
+        <v>45.984</v>
       </c>
       <c r="E34" t="n">
-        <v>2.371</v>
+        <v>-1.305</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000792</v>
+        <v>0.00000000000000000000000000000000000000000000000000021</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C35" t="n">
-        <v>50.882</v>
+        <v>9.07</v>
       </c>
       <c r="D35" t="n">
-        <v>18.08</v>
+        <v>20.554</v>
       </c>
       <c r="E35" t="n">
-        <v>1.443</v>
+        <v>-1.098</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000164</v>
+        <v>0.000000000000000246</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C36" t="n">
-        <v>6.2</v>
+        <v>24.609</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03</v>
+        <v>54.57</v>
       </c>
       <c r="E36" t="n">
-        <v>2.805</v>
+        <v>-1.118</v>
       </c>
       <c r="F36" t="n">
-        <v>0.000000000000000000000000000000000000000000000000829</v>
+        <v>0.000000000000000000000000000000000000000000000000000063</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C37" t="n">
-        <v>4.61</v>
+        <v>7.67</v>
       </c>
       <c r="D37" t="n">
-        <v>0.12</v>
+        <v>21.41</v>
       </c>
       <c r="E37" t="n">
-        <v>2.325</v>
+        <v>-1.37</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000591</v>
+        <v>0.00000000000000000000000000000000000545</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C38" t="n">
-        <v>8.19</v>
+        <v>13.85</v>
       </c>
       <c r="D38" t="n">
-        <v>3.31</v>
+        <v>38.019</v>
       </c>
       <c r="E38" t="n">
-        <v>1.092</v>
+        <v>-1.394</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00000000000000000000000000000000000000000000000115</v>
+        <v>0.000000000000000000000000000000000104</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C39" t="n">
-        <v>12.37</v>
+        <v>1.52</v>
       </c>
       <c r="D39" t="n">
-        <v>2.21</v>
+        <v>10.93</v>
       </c>
       <c r="E39" t="n">
-        <v>2.058</v>
+        <v>-2.243</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000201</v>
+        <v>0.0000000000103</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="C40" t="n">
-        <v>2.2</v>
+        <v>9.66</v>
       </c>
       <c r="D40" t="n">
-        <v>0.165</v>
+        <v>24.48</v>
       </c>
       <c r="E40" t="n">
-        <v>1.458</v>
+        <v>-1.257</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000372</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000217</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C41" t="n">
-        <v>21.96</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>7.755</v>
+        <v>7.885</v>
       </c>
       <c r="E41" t="n">
-        <v>1.391</v>
+        <v>-3.151</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0000000000000000000000000000000000000197</v>
+        <v>0.000000000000000000000000000000135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>